<commit_message>
progress on slides, presentation notes, and assessment
</commit_message>
<xml_diff>
--- a/final-deliverables/deliverables-checklist.xlsx
+++ b/final-deliverables/deliverables-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jasmine\Documents\UIUC\Fall 2019\IS590 Open Data Mashups\final-deliverables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EB4A74E-4C4F-4A9E-B4E4-066F7D8BC974}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B36EC173-88B4-46E8-8C60-D66AD7789F05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{CA5DA797-928C-4257-AB81-5FADF6247F41}"/>
   </bookViews>
@@ -162,15 +162,9 @@
     <t>pretty sure this is done!</t>
   </si>
   <si>
-    <t>some slides are done</t>
-  </si>
-  <si>
     <t>IT IS DONE</t>
   </si>
   <si>
-    <t>the file exists and has a sentence</t>
-  </si>
-  <si>
     <t>it's done, dummy, leave it alone</t>
   </si>
   <si>
@@ -178,6 +172,12 @@
   </si>
   <si>
     <t>I have a script to go with my slides, haven't timed that shit tho</t>
+  </si>
+  <si>
+    <t>the file exists and is almost done</t>
+  </si>
+  <si>
+    <t>slides are done</t>
   </si>
 </sst>
 </file>
@@ -670,8 +670,8 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="40" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -711,41 +711,41 @@
         <v>19</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="6" customFormat="1" ht="167.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" s="6" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="6" customFormat="1" ht="167.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" s="6" customFormat="1" ht="84.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>36</v>
-      </c>
       <c r="C4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E4" s="1">
         <v>1</v>
@@ -779,7 +779,7 @@
         <v>19</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="1">
         <v>2</v>
@@ -796,7 +796,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E7" s="10">
         <v>2</v>
@@ -820,7 +820,7 @@
         <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="1">
         <v>2</v>
@@ -955,7 +955,7 @@
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="E7:E8"/>
   </mergeCells>
-  <conditionalFormatting sqref="E2:E7 E9:E16">
+  <conditionalFormatting sqref="E9:E16 E2:E7">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>